<commit_message>
Update after calender changes
</commit_message>
<xml_diff>
--- a/2021/2021FSAdates.xlsx
+++ b/2021/2021FSAdates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2021\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA52095-EA7B-4B07-8563-1728CB0E0B8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B207B571-9D5E-4B40-AFB3-FECBAF5C6D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12285" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16965" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -106,9 +106,6 @@
     <t>U11</t>
   </si>
   <si>
-    <t>FCC</t>
-  </si>
-  <si>
     <t>BK</t>
   </si>
   <si>
@@ -124,18 +121,6 @@
     <t>U1720</t>
   </si>
   <si>
-    <t>U14T</t>
-  </si>
-  <si>
-    <t>U12</t>
-  </si>
-  <si>
-    <t>U14</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
     <t>10:00</t>
   </si>
   <si>
@@ -157,9 +142,6 @@
     <t>13:00</t>
   </si>
   <si>
-    <t>09:00</t>
-  </si>
-  <si>
     <t>09:45</t>
   </si>
   <si>
@@ -193,10 +175,13 @@
     <t>09:30</t>
   </si>
   <si>
-    <t>08:30</t>
-  </si>
-  <si>
     <t>10:30</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>SASchools</t>
   </si>
 </sst>
 </file>
@@ -312,12 +297,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I93" tableType="xml" totalsRowShown="0" connectionId="2">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I93">
-    <sortCondition ref="A2:A93"/>
-    <sortCondition ref="F2:F93"/>
-    <sortCondition ref="B2:B93"/>
-    <sortCondition ref="C2:C93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I92" tableType="xml" totalsRowShown="0" connectionId="2">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I92">
+    <sortCondition ref="A8:A92"/>
+    <sortCondition ref="F8:F92"/>
+    <sortCondition ref="B8:B92"/>
+    <sortCondition ref="C8:C92"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Date" name="Date">
@@ -649,7 +634,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:L92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -705,10 +690,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20210314</v>
+        <v>20210228</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -720,10 +705,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>19</v>
@@ -731,22 +716,22 @@
       <c r="I2" s="3"/>
       <c r="K2" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210314U13BE</v>
+        <v>20210228OME</v>
       </c>
       <c r="L2" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210314U13GE</v>
+        <v>20210228OWE</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>20210314</v>
+        <v>20210228</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -758,7 +743,7 @@
         <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>19</v>
@@ -766,19 +751,19 @@
       <c r="I3" s="3"/>
       <c r="K3" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210314U15MF</v>
+        <v>20210228OMS</v>
       </c>
       <c r="L3" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210314U15WF</v>
+        <v>20210228OWS</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>20210314</v>
+        <v>20210228</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -790,10 +775,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>19</v>
@@ -801,22 +786,22 @@
       <c r="I4" s="3"/>
       <c r="K4" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210314U11BF</v>
+        <v>20210228VMF</v>
       </c>
       <c r="L4" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210314U11GF</v>
+        <v>20210228VWF</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>20210314</v>
+        <v>20210228</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -825,10 +810,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>19</v>
@@ -836,22 +821,22 @@
       <c r="I5" s="3"/>
       <c r="K5" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210314U11BE</v>
+        <v>20210228OMF</v>
       </c>
       <c r="L5" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210314U11GE</v>
+        <v>20210228OWF</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>20210314</v>
+        <v>20210228</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -860,10 +845,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>19</v>
@@ -871,22 +856,22 @@
       <c r="I6" s="3"/>
       <c r="K6" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210314U13BF</v>
+        <v>20210228VME</v>
       </c>
       <c r="L6" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210314U13GF</v>
+        <v>20210228VWE</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>20210314</v>
+        <v>20210228</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -895,10 +880,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>19</v>
@@ -906,19 +891,19 @@
       <c r="I7" s="3"/>
       <c r="K7" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210314U15ME</v>
+        <v>20210228VMS</v>
       </c>
       <c r="L7" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210314U15WE</v>
+        <v>20210228VWS</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>20210321</v>
+        <v>20210314</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -930,10 +915,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>19</v>
@@ -941,22 +926,22 @@
       <c r="I8" s="3"/>
       <c r="K8" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210321OME</v>
+        <v>20210314U13BE</v>
       </c>
       <c r="L8" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210321OWE</v>
+        <v>20210314U13GE</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>20210321</v>
+        <v>20210314</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -965,10 +950,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>19</v>
@@ -976,19 +961,19 @@
       <c r="I9" s="3"/>
       <c r="K9" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210321OMS</v>
+        <v>20210314U15MF</v>
       </c>
       <c r="L9" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210321OWS</v>
+        <v>20210314U15WF</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>20210321</v>
+        <v>20210314</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -1000,10 +985,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>19</v>
@@ -1011,22 +996,22 @@
       <c r="I10" s="3"/>
       <c r="K10" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210321VMF</v>
+        <v>20210314U11BF</v>
       </c>
       <c r="L10" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210321VWF</v>
+        <v>20210314U11GF</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>20210321</v>
+        <v>20210314</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1035,10 +1020,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>19</v>
@@ -1046,22 +1031,22 @@
       <c r="I11" s="3"/>
       <c r="K11" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210321OMF</v>
+        <v>20210314U11BE</v>
       </c>
       <c r="L11" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210321OWF</v>
+        <v>20210314U11GE</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>20210321</v>
+        <v>20210314</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1070,10 +1055,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>19</v>
@@ -1081,22 +1066,22 @@
       <c r="I12" s="3"/>
       <c r="K12" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210321VME</v>
+        <v>20210314U13BF</v>
       </c>
       <c r="L12" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210321VWE</v>
+        <v>20210314U13GF</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>20210321</v>
+        <v>20210314</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1105,10 +1090,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>19</v>
@@ -1116,22 +1101,22 @@
       <c r="I13" s="3"/>
       <c r="K13" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210321VMS</v>
+        <v>20210314U15ME</v>
       </c>
       <c r="L13" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210321VWS</v>
+        <v>20210314U15WE</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>20210501</v>
+        <v>20210321</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1140,33 +1125,33 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I14" s="3"/>
       <c r="K14" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210501U10MF</v>
+        <v>20210321OME</v>
       </c>
       <c r="L14" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210501U10WF</v>
+        <v>20210321OWE</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>20210501</v>
+        <v>20210321</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1178,27 +1163,27 @@
         <v>31</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I15" s="3"/>
       <c r="K15" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210501U12ME</v>
+        <v>20210321OMS</v>
       </c>
       <c r="L15" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210501U12WE</v>
+        <v>20210321OWS</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>20210501</v>
+        <v>20210321</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
@@ -1210,33 +1195,33 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I16" s="3"/>
       <c r="K16" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210501U12MF</v>
+        <v>20210321VMF</v>
       </c>
       <c r="L16" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210501U12WF</v>
+        <v>20210321VWF</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>20210501</v>
+        <v>20210321</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1245,30 +1230,30 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I17" s="3"/>
       <c r="K17" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210501U14ME</v>
+        <v>20210321OMF</v>
       </c>
       <c r="L17" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210501U14WE</v>
+        <v>20210321OWF</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>20210502</v>
+        <v>20210321</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -1280,33 +1265,33 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I18" s="3"/>
       <c r="K18" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210502U14TME</v>
+        <v>20210321VME</v>
       </c>
       <c r="L18" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210502U14TWE</v>
+        <v>20210321VWE</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>20210502</v>
+        <v>20210321</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1315,22 +1300,22 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I19" s="3"/>
       <c r="K19" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210502U14TMF</v>
+        <v>20210321VMS</v>
       </c>
       <c r="L19" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210502U14TWF</v>
+        <v>20210321VWS</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1338,10 +1323,10 @@
         <v>20210502</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1350,22 +1335,22 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I20" s="3"/>
       <c r="K20" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210502U14TMS</v>
+        <v>20210502U1720MF</v>
       </c>
       <c r="L20" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210502U14TWS</v>
+        <v>20210502U1720WF</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1373,10 +1358,10 @@
         <v>20210502</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1385,22 +1370,22 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I21" s="3"/>
       <c r="K21" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210502U14MF</v>
+        <v>20210502OBME</v>
       </c>
       <c r="L21" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210502U14WF</v>
+        <v>20210502OBWE</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1408,7 +1393,7 @@
         <v>20210502</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -1420,30 +1405,30 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="I22" s="3"/>
       <c r="K22" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210502U14MS</v>
+        <v>20210502U1720MS</v>
       </c>
       <c r="L22" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210502U14WS</v>
+        <v>20210502U1720WS</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>20210516</v>
+        <v>20210502</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>11</v>
@@ -1455,10 +1440,10 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>19</v>
@@ -1466,19 +1451,19 @@
       <c r="I23" s="3"/>
       <c r="K23" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210516U1720MF</v>
+        <v>20210502OBMF</v>
       </c>
       <c r="L23" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210516U1720WF</v>
+        <v>20210502OBWF</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>20210516</v>
+        <v>20210502</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -1490,10 +1475,10 @@
         <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>19</v>
@@ -1501,19 +1486,19 @@
       <c r="I24" s="3"/>
       <c r="K24" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210516OBME</v>
+        <v>20210502U1720ME</v>
       </c>
       <c r="L24" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210516OBWE</v>
+        <v>20210502U1720WE</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>20210516</v>
+        <v>20210502</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
@@ -1525,10 +1510,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>19</v>
@@ -1536,11 +1521,11 @@
       <c r="I25" s="3"/>
       <c r="K25" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210516U1720MS</v>
+        <v>20210502OBMS</v>
       </c>
       <c r="L25" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210516U1720WS</v>
+        <v>20210502OBWS</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1548,10 +1533,10 @@
         <v>20210516</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1560,10 +1545,10 @@
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>19</v>
@@ -1571,11 +1556,11 @@
       <c r="I26" s="3"/>
       <c r="K26" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210516OBMF</v>
+        <v>20210516U13BE</v>
       </c>
       <c r="L26" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210516OBWF</v>
+        <v>20210516U13GE</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1583,22 +1568,22 @@
         <v>20210516</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>19</v>
@@ -1606,11 +1591,11 @@
       <c r="I27" s="3"/>
       <c r="K27" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210516U1720ME</v>
+        <v>20210516U15MF</v>
       </c>
       <c r="L27" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210516U1720WE</v>
+        <v>20210516U15WF</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1618,10 +1603,10 @@
         <v>20210516</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1630,10 +1615,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>19</v>
@@ -1641,19 +1626,19 @@
       <c r="I28" s="3"/>
       <c r="K28" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210516OBMS</v>
+        <v>20210516U11BF</v>
       </c>
       <c r="L28" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210516OBWS</v>
+        <v>20210516U11GF</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>20210530</v>
+        <v>20210516</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>12</v>
@@ -1665,33 +1650,33 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I29" s="3"/>
       <c r="K29" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210530OME</v>
+        <v>20210516U11BE</v>
       </c>
       <c r="L29" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210530OWE</v>
+        <v>20210516U11GE</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>20210530</v>
+        <v>20210516</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1700,33 +1685,33 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I30" s="3"/>
       <c r="K30" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210530OMS</v>
+        <v>20210516U13BF</v>
       </c>
       <c r="L30" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210530OWS</v>
+        <v>20210516U13GF</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>20210530</v>
+        <v>20210516</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1735,10 +1720,10 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>19</v>
@@ -1746,11 +1731,11 @@
       <c r="I31" s="3"/>
       <c r="K31" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210530VMF</v>
+        <v>20210516U15ME</v>
       </c>
       <c r="L31" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210530VWF</v>
+        <v>20210516U15WE</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1761,7 +1746,7 @@
         <v>18</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1770,22 +1755,22 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I32" s="3"/>
       <c r="K32" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210530OMF</v>
+        <v>20210530OME</v>
       </c>
       <c r="L32" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210530OWF</v>
+        <v>20210530OWE</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1793,10 +1778,10 @@
         <v>20210530</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1805,22 +1790,22 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="H33" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I33" s="3"/>
       <c r="K33" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210530VME</v>
+        <v>20210530OMS</v>
       </c>
       <c r="L33" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210530VWE</v>
+        <v>20210530OWS</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1831,7 +1816,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1840,10 +1825,10 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>19</v>
@@ -1851,19 +1836,19 @@
       <c r="I34" s="3"/>
       <c r="K34" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210530VMS</v>
+        <v>20210530VMF</v>
       </c>
       <c r="L34" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210530VWS</v>
+        <v>20210530VWF</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>20210627</v>
+        <v>20210530</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>11</v>
@@ -1875,30 +1860,30 @@
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I35" s="3"/>
       <c r="K35" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210627U1720MF</v>
+        <v>20210530OMF</v>
       </c>
       <c r="L35" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210627U1720WF</v>
+        <v>20210530OWF</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>20210627</v>
+        <v>20210530</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>12</v>
@@ -1913,7 +1898,7 @@
         <v>32</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>19</v>
@@ -1921,19 +1906,19 @@
       <c r="I36" s="3"/>
       <c r="K36" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210627OBME</v>
+        <v>20210530VME</v>
       </c>
       <c r="L36" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210627OBWE</v>
+        <v>20210530VWE</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>20210627</v>
+        <v>20210530</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>13</v>
@@ -1945,10 +1930,10 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>19</v>
@@ -1956,11 +1941,11 @@
       <c r="I37" s="3"/>
       <c r="K37" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210627U1720MS</v>
+        <v>20210530VMS</v>
       </c>
       <c r="L37" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210627U1720WS</v>
+        <v>20210530VWS</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -1968,7 +1953,7 @@
         <v>20210627</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>11</v>
@@ -1980,10 +1965,10 @@
         <v>1</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>19</v>
@@ -1991,11 +1976,11 @@
       <c r="I38" s="3"/>
       <c r="K38" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210627OBMF</v>
+        <v>20210627U1720MF</v>
       </c>
       <c r="L38" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210627OBWF</v>
+        <v>20210627U1720WF</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2003,7 +1988,7 @@
         <v>20210627</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>12</v>
@@ -2015,10 +2000,10 @@
         <v>1</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>19</v>
@@ -2026,11 +2011,11 @@
       <c r="I39" s="3"/>
       <c r="K39" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210627U1720ME</v>
+        <v>20210627OBME</v>
       </c>
       <c r="L39" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210627U1720WE</v>
+        <v>20210627OBWE</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2038,7 +2023,7 @@
         <v>20210627</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -2050,10 +2035,10 @@
         <v>1</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>19</v>
@@ -2061,22 +2046,22 @@
       <c r="I40" s="3"/>
       <c r="K40" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210627OBMS</v>
+        <v>20210627U1720MS</v>
       </c>
       <c r="L40" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210627OBWS</v>
+        <v>20210627U1720WS</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>20210725</v>
+        <v>20210627</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2085,33 +2070,33 @@
         <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="1"/>
+      <c r="I41" s="3"/>
       <c r="K41" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210725U13BE</v>
+        <v>20210627OBMF</v>
       </c>
       <c r="L41" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210725U13GE</v>
+        <v>20210627OBWF</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>20210725</v>
+        <v>20210627</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2120,33 +2105,33 @@
         <v>1</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="1"/>
+      <c r="I42" s="3"/>
       <c r="K42" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210725U15MF</v>
+        <v>20210627U1720ME</v>
       </c>
       <c r="L42" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210725U15WF</v>
+        <v>20210627U1720WE</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>20210725</v>
+        <v>20210627</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2155,30 +2140,30 @@
         <v>1</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I43" s="1"/>
+      <c r="I43" s="3"/>
       <c r="K43" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210725U11BF</v>
+        <v>20210627OBMS</v>
       </c>
       <c r="L43" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210725U11GF</v>
+        <v>20210627OBWS</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>20210725</v>
+        <v>20210801</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>12</v>
@@ -2190,10 +2175,10 @@
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>19</v>
@@ -2201,19 +2186,19 @@
       <c r="I44" s="1"/>
       <c r="K44" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210725U11BE</v>
+        <v>20210801U13BE</v>
       </c>
       <c r="L44" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210725U11GE</v>
+        <v>20210801U13GE</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>20210725</v>
+        <v>20210801</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>11</v>
@@ -2225,10 +2210,10 @@
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>19</v>
@@ -2236,22 +2221,22 @@
       <c r="I45" s="1"/>
       <c r="K45" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210725U13BF</v>
+        <v>20210801U15MF</v>
       </c>
       <c r="L45" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210725U13GF</v>
+        <v>20210801U15WF</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>20210725</v>
+        <v>20210801</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2260,10 +2245,10 @@
         <v>1</v>
       </c>
       <c r="F46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>19</v>
@@ -2271,19 +2256,19 @@
       <c r="I46" s="1"/>
       <c r="K46" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210725U15ME</v>
+        <v>20210801U11BF</v>
       </c>
       <c r="L46" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210725U15WE</v>
+        <v>20210801U11GF</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>12</v>
@@ -2295,33 +2280,33 @@
         <v>1</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I47" s="1"/>
       <c r="K47" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815OME</v>
+        <v>20210801U11BE</v>
       </c>
       <c r="L47" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815OWE</v>
+        <v>20210801U11GE</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2330,33 +2315,33 @@
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I48" s="1"/>
       <c r="K48" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815OMS</v>
+        <v>20210801U13BF</v>
       </c>
       <c r="L48" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815OWS</v>
+        <v>20210801U13GF</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2365,10 +2350,10 @@
         <v>1</v>
       </c>
       <c r="F49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>19</v>
@@ -2376,11 +2361,11 @@
       <c r="I49" s="1"/>
       <c r="K49" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815VMF</v>
+        <v>20210801U15ME</v>
       </c>
       <c r="L49" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815VWF</v>
+        <v>20210801U15WE</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2391,7 +2376,7 @@
         <v>18</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2400,22 +2385,22 @@
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I50" s="1"/>
       <c r="K50" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815OMF</v>
+        <v>20210815OME</v>
       </c>
       <c r="L50" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815OWF</v>
+        <v>20210815OWE</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2423,10 +2408,10 @@
         <v>20210815</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2435,22 +2420,22 @@
         <v>1</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="H51" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I51" s="1"/>
       <c r="K51" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815VME</v>
+        <v>20210815OMS</v>
       </c>
       <c r="L51" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815VWE</v>
+        <v>20210815OWS</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2461,7 +2446,7 @@
         <v>9</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2470,10 +2455,10 @@
         <v>1</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>19</v>
@@ -2481,19 +2466,19 @@
       <c r="I52" s="1"/>
       <c r="K52" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815VMS</v>
+        <v>20210815VMF</v>
       </c>
       <c r="L52" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815VWS</v>
+        <v>20210815VWF</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>20210905</v>
+        <v>20210815</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -2505,30 +2490,30 @@
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I53" s="1"/>
       <c r="K53" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905U1720MF</v>
+        <v>20210815OMF</v>
       </c>
       <c r="L53" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905U1720WF</v>
+        <v>20210815OWF</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>20210905</v>
+        <v>20210815</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>12</v>
@@ -2543,27 +2528,27 @@
         <v>32</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I54" s="1"/>
       <c r="K54" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905OBME</v>
+        <v>20210815VME</v>
       </c>
       <c r="L54" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905OBWE</v>
+        <v>20210815VWE</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>20210905</v>
+        <v>20210815</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>13</v>
@@ -2575,30 +2560,30 @@
         <v>1</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I55" s="1"/>
       <c r="K55" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905U1720MS</v>
+        <v>20210815VMS</v>
       </c>
       <c r="L55" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905U1720WS</v>
+        <v>20210815VWS</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>20210905</v>
+        <v>20210822</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>11</v>
@@ -2610,22 +2595,22 @@
         <v>1</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="I56" s="1"/>
       <c r="K56" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905OBMF</v>
+        <v>20210822U17MF</v>
       </c>
       <c r="L56" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905OBWF</v>
+        <v>20210822U17WF</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -2633,34 +2618,34 @@
         <v>20210905</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="G57" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I57" s="1"/>
       <c r="K57" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905U1720ME</v>
+        <v>20210905U1720MF</v>
       </c>
       <c r="L57" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905U1720WE</v>
+        <v>20210905U1720WF</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -2671,7 +2656,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2680,33 +2665,33 @@
         <v>1</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I58" s="1"/>
       <c r="K58" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905OBMS</v>
+        <v>20210905OBME</v>
       </c>
       <c r="L58" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905OBWS</v>
+        <v>20210905OBWE</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>20210919</v>
+        <v>20210905</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2715,33 +2700,33 @@
         <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I59" s="1"/>
       <c r="K59" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210919OME</v>
+        <v>20210905U1720MS</v>
       </c>
       <c r="L59" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210919OWE</v>
+        <v>20210905U1720WS</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>20210919</v>
+        <v>20210905</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2750,33 +2735,33 @@
         <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H60" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I60" s="1"/>
       <c r="K60" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210919OMS</v>
+        <v>20210905OBMF</v>
       </c>
       <c r="L60" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210919OWS</v>
+        <v>20210905OBWF</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>20210919</v>
+        <v>20210905</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2785,33 +2770,33 @@
         <v>1</v>
       </c>
       <c r="F61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G61" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H61" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I61" s="1"/>
       <c r="K61" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210919VMF</v>
+        <v>20210905U1720ME</v>
       </c>
       <c r="L61" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210919VWF</v>
+        <v>20210905U1720WE</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>20210919</v>
+        <v>20210905</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2820,22 +2805,22 @@
         <v>1</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I62" s="1"/>
       <c r="K62" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210919OMF</v>
+        <v>20210905OBMS</v>
       </c>
       <c r="L62" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210919OWF</v>
+        <v>20210905OBWS</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -2843,45 +2828,45 @@
         <v>20210919</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="I63" s="1"/>
       <c r="K63" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210919VME</v>
+        <v>20210919U17TF</v>
       </c>
       <c r="L63" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210919VWE</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>20210919</v>
+        <v>20211017</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2890,22 +2875,22 @@
         <v>1</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I64" s="1"/>
       <c r="K64" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210919VMS</v>
+        <v>20211017OME</v>
       </c>
       <c r="L64" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210919VWS</v>
+        <v>20211017OWE</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -2916,7 +2901,7 @@
         <v>18</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2928,19 +2913,19 @@
         <v>31</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I65" s="1"/>
       <c r="K65" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017OME</v>
+        <v>20211017OMS</v>
       </c>
       <c r="L65" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017OWE</v>
+        <v>20211017OWS</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -2948,10 +2933,10 @@
         <v>20211017</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2960,22 +2945,22 @@
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I66" s="1"/>
       <c r="K66" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017OMS</v>
+        <v>20211017VMF</v>
       </c>
       <c r="L66" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017OWS</v>
+        <v>20211017VWF</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -2983,7 +2968,7 @@
         <v>20211017</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>11</v>
@@ -2995,22 +2980,22 @@
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I67" s="1"/>
       <c r="K67" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017VMF</v>
+        <v>20211017OMF</v>
       </c>
       <c r="L67" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017VWF</v>
+        <v>20211017OWF</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3018,10 +3003,10 @@
         <v>20211017</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -3030,22 +3015,22 @@
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I68" s="1"/>
       <c r="K68" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017OMF</v>
+        <v>20211017VME</v>
       </c>
       <c r="L68" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017OWF</v>
+        <v>20211017VWE</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3056,7 +3041,7 @@
         <v>9</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3065,33 +3050,33 @@
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I69" s="1"/>
       <c r="K69" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017VME</v>
+        <v>20211017VMS</v>
       </c>
       <c r="L69" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017VWE</v>
+        <v>20211017VWS</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>20211017</v>
+        <v>20211024</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -3100,22 +3085,22 @@
         <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I70" s="1"/>
       <c r="K70" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017VMS</v>
+        <v>20211024U1720MF</v>
       </c>
       <c r="L70" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017VWS</v>
+        <v>20211024U1720WF</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3123,10 +3108,10 @@
         <v>20211024</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -3135,10 +3120,10 @@
         <v>1</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>19</v>
@@ -3146,11 +3131,11 @@
       <c r="I71" s="1"/>
       <c r="K71" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024U1720MF</v>
+        <v>20211024OBME</v>
       </c>
       <c r="L71" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024U1720WF</v>
+        <v>20211024OBWE</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -3158,10 +3143,10 @@
         <v>20211024</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3170,10 +3155,10 @@
         <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>19</v>
@@ -3181,11 +3166,11 @@
       <c r="I72" s="1"/>
       <c r="K72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024OBME</v>
+        <v>20211024U1720MS</v>
       </c>
       <c r="L72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024OBWE</v>
+        <v>20211024U1720WS</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -3193,10 +3178,10 @@
         <v>20211024</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -3205,10 +3190,10 @@
         <v>1</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>19</v>
@@ -3216,11 +3201,11 @@
       <c r="I73" s="1"/>
       <c r="K73" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024U1720MS</v>
+        <v>20211024OBMF</v>
       </c>
       <c r="L73" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024U1720WS</v>
+        <v>20211024OBWF</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3228,10 +3213,10 @@
         <v>20211024</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -3240,10 +3225,10 @@
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>19</v>
@@ -3251,11 +3236,11 @@
       <c r="I74" s="1"/>
       <c r="K74" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024OBMF</v>
+        <v>20211024U1720ME</v>
       </c>
       <c r="L74" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024OBWF</v>
+        <v>20211024U1720WE</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3263,10 +3248,10 @@
         <v>20211024</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3275,10 +3260,10 @@
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>19</v>
@@ -3286,22 +3271,22 @@
       <c r="I75" s="1"/>
       <c r="K75" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024U1720ME</v>
+        <v>20211024OBMS</v>
       </c>
       <c r="L75" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024U1720WE</v>
+        <v>20211024OBWS</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>20211024</v>
+        <v>20211107</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3310,22 +3295,22 @@
         <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I76" s="1"/>
       <c r="K76" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024OBMS</v>
+        <v>20211107U13BE</v>
       </c>
       <c r="L76" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024OBWS</v>
+        <v>20211107U13GE</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -3333,10 +3318,10 @@
         <v>20211107</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -3345,22 +3330,22 @@
         <v>1</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I77" s="1"/>
       <c r="K77" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U13BE</v>
+        <v>20211107U15MF</v>
       </c>
       <c r="L77" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U13GE</v>
+        <v>20211107U15WF</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3368,7 +3353,7 @@
         <v>20211107</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>11</v>
@@ -3380,22 +3365,22 @@
         <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I78" s="1"/>
       <c r="K78" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U15MF</v>
+        <v>20211107U11BF</v>
       </c>
       <c r="L78" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U15WF</v>
+        <v>20211107U11GF</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -3406,7 +3391,7 @@
         <v>20</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -3418,19 +3403,19 @@
         <v>32</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I79" s="1"/>
       <c r="K79" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U11BF</v>
+        <v>20211107U11BE</v>
       </c>
       <c r="L79" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U11GF</v>
+        <v>20211107U11GE</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -3438,10 +3423,10 @@
         <v>20211107</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3450,22 +3435,22 @@
         <v>1</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I80" s="1"/>
       <c r="K80" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U11BE</v>
+        <v>20211107U13BF</v>
       </c>
       <c r="L80" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U11GE</v>
+        <v>20211107U13GF</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -3473,10 +3458,10 @@
         <v>20211107</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3485,30 +3470,30 @@
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I81" s="1"/>
       <c r="K81" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U13BF</v>
+        <v>20211107U15ME</v>
       </c>
       <c r="L81" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U13GF</v>
+        <v>20211107U15WE</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>20211107</v>
+        <v>20211121</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>12</v>
@@ -3520,33 +3505,33 @@
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I82" s="1"/>
       <c r="K82" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U15ME</v>
+        <v>20211121OME</v>
       </c>
       <c r="L82" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U15WE</v>
+        <v>20211121OWE</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>20211114</v>
+        <v>20211121</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -3558,30 +3543,30 @@
         <v>31</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I83" s="1"/>
       <c r="K83" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211114OME</v>
+        <v>20211121OMS</v>
       </c>
       <c r="L83" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211114OWE</v>
+        <v>20211121OWS</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>20211114</v>
+        <v>20211121</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -3590,30 +3575,30 @@
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I84" s="1"/>
       <c r="K84" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211114OMS</v>
+        <v>20211121VMF</v>
       </c>
       <c r="L84" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211114OWS</v>
+        <v>20211121VWF</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>20211114</v>
+        <v>20211121</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>11</v>
@@ -3625,33 +3610,33 @@
         <v>1</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I85" s="1"/>
       <c r="K85" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211114VMF</v>
+        <v>20211121OMF</v>
       </c>
       <c r="L85" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211114VWF</v>
+        <v>20211121OWF</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>20211114</v>
+        <v>20211121</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -3660,33 +3645,33 @@
         <v>1</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I86" s="1"/>
       <c r="K86" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211114OMF</v>
+        <v>20211121VME</v>
       </c>
       <c r="L86" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211114OWF</v>
+        <v>20211121VWE</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>20211114</v>
+        <v>20211121</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -3695,68 +3680,68 @@
         <v>1</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I87" s="1"/>
       <c r="K87" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211114VME</v>
+        <v>20211121VMS</v>
       </c>
       <c r="L87" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211114VWE</v>
+        <v>20211121VWS</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>20211114</v>
+        <v>20211128</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I88" s="1"/>
       <c r="K88" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211114VMS</v>
+        <v>20211128U13TE</v>
       </c>
       <c r="L88" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211114VWS</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>20211121</v>
+        <v>20211128</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -3765,10 +3750,10 @@
         <v>0</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>19</v>
@@ -3776,7 +3761,7 @@
       <c r="I89" s="1"/>
       <c r="K89" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121U13TE</v>
+        <v>20211128U13TF</v>
       </c>
       <c r="L89" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
@@ -3785,13 +3770,13 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>20211121</v>
+        <v>20211128</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -3800,10 +3785,10 @@
         <v>0</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>19</v>
@@ -3811,7 +3796,7 @@
       <c r="I90" s="1"/>
       <c r="K90" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121U13TF</v>
+        <v>20211128U17TE</v>
       </c>
       <c r="L90" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
@@ -3820,13 +3805,13 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>20211121</v>
+        <v>20211128</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -3835,10 +3820,10 @@
         <v>0</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>19</v>
@@ -3846,7 +3831,7 @@
       <c r="I91" s="1"/>
       <c r="K91" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121U17TE</v>
+        <v>20211128U17TF</v>
       </c>
       <c r="L91" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
@@ -3855,14 +3840,12 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>20211121</v>
+        <v>20211128</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C92" s="1"/>
       <c r="D92">
         <v>0</v>
       </c>
@@ -3873,7 +3856,7 @@
         <v>32</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>19</v>
@@ -3881,42 +3864,9 @@
       <c r="I92" s="1"/>
       <c r="K92" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121U17TF</v>
+        <v>20211128OT</v>
       </c>
       <c r="L92" t="str">
-        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>20211121</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C93" s="1"/>
-      <c r="D93">
-        <v>0</v>
-      </c>
-      <c r="E93">
-        <v>0</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I93" s="1"/>
-      <c r="K93" t="str">
-        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121OT</v>
-      </c>
-      <c r="L93" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
         <v>N/A</v>
       </c>

</xml_diff>

<commit_message>
Update for cancelled events
</commit_message>
<xml_diff>
--- a/2021/2021FSAdates.xlsx
+++ b/2021/2021FSAdates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2021\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FSA\Dropbox\Competitions\2021\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B207B571-9D5E-4B40-AFB3-FECBAF5C6D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544E055F-2AC6-4494-8DF7-4C72F233A8EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16965" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -769,7 +769,7 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -786,11 +786,11 @@
       <c r="I4" s="3"/>
       <c r="K4" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210228VMF</v>
+        <v>N/A</v>
       </c>
       <c r="L4" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210228VWF</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -874,7 +874,7 @@
         <v>13</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -891,11 +891,11 @@
       <c r="I7" s="3"/>
       <c r="K7" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210228VMS</v>
+        <v>N/A</v>
       </c>
       <c r="L7" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210228VWS</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updae to results dates for calendar changes
</commit_message>
<xml_diff>
--- a/2021/2021FSAdates.xlsx
+++ b/2021/2021FSAdates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FSA\Dropbox\Competitions\2021\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2021\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620643C-669A-4B8F-8037-2C041481CB36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE932691-80A8-4A53-A62B-43E7E5F5FDC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -297,12 +297,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I101" tableType="xml" totalsRowShown="0" connectionId="2">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I101">
-    <sortCondition ref="A2:A101"/>
-    <sortCondition ref="F2:F101"/>
-    <sortCondition ref="B2:B101"/>
-    <sortCondition ref="C2:C101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I107" tableType="xml" totalsRowShown="0" connectionId="2">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I107">
+    <sortCondition ref="A2:A107"/>
+    <sortCondition ref="F2:F107"/>
+    <sortCondition ref="B2:B107"/>
+    <sortCondition ref="C2:C107"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Date" name="Date">
@@ -634,28 +634,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -690,7 +690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20210228</v>
       </c>
@@ -725,7 +725,7 @@
         <v>20210228OWE</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20210228</v>
       </c>
@@ -760,7 +760,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -795,7 +795,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -830,7 +830,7 @@
         <v>20210228OWF</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -865,7 +865,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -900,7 +900,7 @@
         <v>20210228VWE</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -935,7 +935,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20210314</v>
       </c>
@@ -970,7 +970,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20210314</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20210314</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>20210314U15WF</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20210314</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20210314</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>20210314U11GF</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20210314</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20210314</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20210314</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20210314</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>20210314U15WE</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20210321</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>20210321OWE</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20210321</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20210321</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>20210321OWS</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20210321</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20210321</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>20210321OWF</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20210321</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20210321</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20210502</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>20210502U1720WF</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20210502</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>20210502OBWE</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20210502</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>20210502U1720WS</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20210502</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>20210502OBWF</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20210502</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>20210502U1720WE</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20210502</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>20210502OBWS</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20210516</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20210516</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>20210516U15WF</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20210516</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20210516</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>20210516U11GF</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20210516</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20210516</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>20210516</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>20210516U13GF</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20210516</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20210523</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>20210523</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>20210523U1720WF</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>20210523</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>20210523</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>20210523OBWE</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>20210523</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>20210523</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>20210523OBWF</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>20210523</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>20210523</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>20210530</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>20210530OWE</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20210530</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>20210530OWS</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20210530</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>20210530VWF</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>20210530</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>20210530OWF</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>20210530</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>20210530VWE</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>20210530</v>
       </c>
@@ -2475,15 +2475,15 @@
         <v>20210530VWS</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>20210801</v>
+        <v>20210627</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2500,95 +2500,95 @@
       <c r="H53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I53" s="1"/>
+      <c r="I53" s="3"/>
       <c r="K53" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210801U13BE</v>
+        <v>20210627U1720MF</v>
       </c>
       <c r="L53" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210801U13GE</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210627U1720WF</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>20210801</v>
+        <v>20210627</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="K54" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20210627OBME</v>
+      </c>
+      <c r="L54" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20210627OBWE</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>20210627</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" s="3"/>
+      <c r="K55" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20210627U1720MS</v>
+      </c>
+      <c r="L55" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20210627U1720WS</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>20210627</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I54" s="1"/>
-      <c r="K54" t="str">
-        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210801U15MF</v>
-      </c>
-      <c r="L54" t="str">
-        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210801U15WF</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>20210801</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" s="1"/>
-      <c r="K55" t="str">
-        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210801U11BF</v>
-      </c>
-      <c r="L55" t="str">
-        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210801U11GF</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>20210801</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2605,25 +2605,25 @@
       <c r="H56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I56" s="1"/>
+      <c r="I56" s="3"/>
       <c r="K56" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210801U11BE</v>
+        <v>20210627OBMF</v>
       </c>
       <c r="L56" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210801U11GE</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210627OBWF</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>20210801</v>
+        <v>20210627</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2632,33 +2632,33 @@
         <v>1</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I57" s="1"/>
+      <c r="I57" s="3"/>
       <c r="K57" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210801U13BF</v>
+        <v>20210627U1720ME</v>
       </c>
       <c r="L57" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210801U13GF</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210627U1720WE</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>20210801</v>
+        <v>20210627</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2667,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>36</v>
@@ -2675,22 +2675,22 @@
       <c r="H58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I58" s="1"/>
+      <c r="I58" s="3"/>
       <c r="K58" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210801U15ME</v>
+        <v>20210627OBMS</v>
       </c>
       <c r="L58" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210801U15WE</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210627OBWS</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>12</v>
@@ -2708,27 +2708,27 @@
         <v>33</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I59" s="1"/>
       <c r="K59" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815OME</v>
+        <v>20210801U13BE</v>
       </c>
       <c r="L59" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815OWE</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210801U13GE</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2737,30 +2737,30 @@
         <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I60" s="1"/>
       <c r="K60" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815OMS</v>
+        <v>20210801U15MF</v>
       </c>
       <c r="L60" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815OWS</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210801U15WF</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>11</v>
@@ -2772,10 +2772,10 @@
         <v>1</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>19</v>
@@ -2783,22 +2783,22 @@
       <c r="I61" s="1"/>
       <c r="K61" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815VMF</v>
+        <v>20210801U11BF</v>
       </c>
       <c r="L61" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815VWF</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210801U11GF</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2813,27 +2813,27 @@
         <v>38</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I62" s="1"/>
       <c r="K62" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815OMF</v>
+        <v>20210801U11BE</v>
       </c>
       <c r="L62" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815OWF</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210801U11GE</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2853,22 +2853,22 @@
       <c r="I63" s="1"/>
       <c r="K63" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815VME</v>
+        <v>20210801U13BF</v>
       </c>
       <c r="L63" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815VWE</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210801U13GF</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>20210815</v>
+        <v>20210801</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2877,10 +2877,10 @@
         <v>1</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>19</v>
@@ -2888,22 +2888,22 @@
       <c r="I64" s="1"/>
       <c r="K64" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210815VMS</v>
+        <v>20210801U15ME</v>
       </c>
       <c r="L64" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210815VWS</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210801U15WE</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>20210822</v>
+        <v>20210815</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2918,27 +2918,27 @@
         <v>33</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="I65" s="1"/>
       <c r="K65" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210822U17MF</v>
+        <v>20210815OME</v>
       </c>
       <c r="L65" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210822U17WF</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210815OWE</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>20210905</v>
+        <v>20210815</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2947,33 +2947,33 @@
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I66" s="1"/>
       <c r="K66" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905U1720MF</v>
+        <v>20210815OMS</v>
       </c>
       <c r="L66" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905U1720WF</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210815OWS</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>20210905</v>
+        <v>20210815</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2982,33 +2982,33 @@
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I67" s="1"/>
       <c r="K67" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905OBME</v>
+        <v>20210815VMF</v>
       </c>
       <c r="L67" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905OBWE</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210815VWF</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>20210905</v>
+        <v>20210815</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -3017,33 +3017,33 @@
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I68" s="1"/>
       <c r="K68" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905U1720MS</v>
+        <v>20210815OMF</v>
       </c>
       <c r="L68" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905U1720WS</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210815OWF</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>20210905</v>
+        <v>20210815</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3052,33 +3052,33 @@
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I69" s="1"/>
       <c r="K69" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905OBMF</v>
+        <v>20210815VME</v>
       </c>
       <c r="L69" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905OBWF</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210815VWE</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>20210905</v>
+        <v>20210815</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -3087,33 +3087,33 @@
         <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I70" s="1"/>
       <c r="K70" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905U1720ME</v>
+        <v>20210815VMS</v>
       </c>
       <c r="L70" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905U1720WE</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210815VWS</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>20210905</v>
+        <v>20210822</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -3122,30 +3122,30 @@
         <v>1</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="I71" s="1"/>
       <c r="K71" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210905OBMS</v>
+        <v>20210822U17MF</v>
       </c>
       <c r="L71" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20210905OBWS</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210822U17WF</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>20210919</v>
+        <v>20210905</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>11</v>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>26</v>
@@ -3163,24 +3163,24 @@
         <v>33</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="I72" s="1"/>
       <c r="K72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20210919U17TF</v>
+        <v>20210905U1720MF</v>
       </c>
       <c r="L72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210905U1720WF</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>20211017</v>
+        <v>20210905</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>12</v>
@@ -3192,10 +3192,10 @@
         <v>1</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>24</v>
@@ -3203,19 +3203,19 @@
       <c r="I73" s="1"/>
       <c r="K73" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017OME</v>
+        <v>20210905OBME</v>
       </c>
       <c r="L73" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017OWE</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210905OBWE</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>20211017</v>
+        <v>20210905</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>13</v>
@@ -3227,10 +3227,10 @@
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>24</v>
@@ -3238,19 +3238,19 @@
       <c r="I74" s="1"/>
       <c r="K74" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017OMS</v>
+        <v>20210905U1720MS</v>
       </c>
       <c r="L74" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017OWS</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210905U1720WS</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>20211017</v>
+        <v>20210905</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>11</v>
@@ -3262,10 +3262,10 @@
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>24</v>
@@ -3273,22 +3273,22 @@
       <c r="I75" s="1"/>
       <c r="K75" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017VMF</v>
+        <v>20210905OBMF</v>
       </c>
       <c r="L75" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017VWF</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210905OBWF</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>20211017</v>
+        <v>20210905</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3297,10 +3297,10 @@
         <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>24</v>
@@ -3308,22 +3308,22 @@
       <c r="I76" s="1"/>
       <c r="K76" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017OMF</v>
+        <v>20210905U1720ME</v>
       </c>
       <c r="L76" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017OWF</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210905U1720WE</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>20211017</v>
+        <v>20210905</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -3332,10 +3332,10 @@
         <v>1</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>24</v>
@@ -3343,57 +3343,57 @@
       <c r="I77" s="1"/>
       <c r="K77" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017VME</v>
+        <v>20210905OBMS</v>
       </c>
       <c r="L77" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017VWE</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20210905OBWS</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>20211017</v>
+        <v>20210919</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="I78" s="1"/>
       <c r="K78" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211017VMS</v>
+        <v>20210919U17TF</v>
       </c>
       <c r="L78" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211017VWS</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>20211024</v>
+        <v>20211017</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -3408,27 +3408,27 @@
         <v>33</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I79" s="1"/>
       <c r="K79" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024U1720MF</v>
+        <v>20211017OME</v>
       </c>
       <c r="L79" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024U1720WF</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211017OWE</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>20211024</v>
+        <v>20211017</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3437,33 +3437,33 @@
         <v>1</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I80" s="1"/>
       <c r="K80" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024OBME</v>
+        <v>20211017OMS</v>
       </c>
       <c r="L80" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024OBWE</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211017OWS</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>20211024</v>
+        <v>20211017</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3472,30 +3472,30 @@
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I81" s="1"/>
       <c r="K81" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024U1720MS</v>
+        <v>20211017VMF</v>
       </c>
       <c r="L81" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024U1720WS</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211017VWF</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>20211024</v>
+        <v>20211017</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>11</v>
@@ -3507,30 +3507,30 @@
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I82" s="1"/>
       <c r="K82" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024OBMF</v>
+        <v>20211017OMF</v>
       </c>
       <c r="L82" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024OBWF</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211017OWF</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>20211024</v>
+        <v>20211017</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>12</v>
@@ -3542,30 +3542,30 @@
         <v>1</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I83" s="1"/>
       <c r="K83" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024U1720ME</v>
+        <v>20211017VME</v>
       </c>
       <c r="L83" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024U1720WE</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211017VWE</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>20211024</v>
+        <v>20211017</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>13</v>
@@ -3577,33 +3577,33 @@
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I84" s="1"/>
       <c r="K84" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211024OBMS</v>
+        <v>20211017VMS</v>
       </c>
       <c r="L84" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211024OBWS</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211017VWS</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>20211107</v>
+        <v>20211024</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -3618,27 +3618,27 @@
         <v>33</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I85" s="1"/>
       <c r="K85" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U13BE</v>
+        <v>20211024U1720MF</v>
       </c>
       <c r="L85" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U13GE</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211024U1720WF</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>20211107</v>
+        <v>20211024</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -3647,33 +3647,33 @@
         <v>1</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I86" s="1"/>
       <c r="K86" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U15MF</v>
+        <v>20211024OBME</v>
       </c>
       <c r="L86" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U15WF</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211024OBWE</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>20211107</v>
+        <v>20211024</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -3682,33 +3682,33 @@
         <v>1</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I87" s="1"/>
       <c r="K87" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U11BF</v>
+        <v>20211024U1720MS</v>
       </c>
       <c r="L87" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U11GF</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211024U1720WS</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>20211107</v>
+        <v>20211024</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -3717,33 +3717,33 @@
         <v>1</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I88" s="1"/>
       <c r="K88" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U11BE</v>
+        <v>20211024OBMF</v>
       </c>
       <c r="L88" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U11GE</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211024OBWF</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>20211107</v>
+        <v>20211024</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -3752,33 +3752,33 @@
         <v>1</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I89" s="1"/>
       <c r="K89" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U13BF</v>
+        <v>20211024U1720ME</v>
       </c>
       <c r="L89" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U13GF</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211024U1720WE</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>20211107</v>
+        <v>20211024</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -3787,30 +3787,30 @@
         <v>1</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I90" s="1"/>
       <c r="K90" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211107U15ME</v>
+        <v>20211024OBMS</v>
       </c>
       <c r="L90" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211107U15WE</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211024OBWS</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>20211121</v>
+        <v>20211107</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>12</v>
@@ -3828,27 +3828,27 @@
         <v>33</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I91" s="1"/>
       <c r="K91" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121OME</v>
+        <v>20211107U13BE</v>
       </c>
       <c r="L91" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211121OWE</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211107U13GE</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>20211121</v>
+        <v>20211107</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -3857,30 +3857,30 @@
         <v>1</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I92" s="1"/>
       <c r="K92" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121OMS</v>
+        <v>20211107U15MF</v>
       </c>
       <c r="L92" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211121OWS</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211107U15WF</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>20211121</v>
+        <v>20211107</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>11</v>
@@ -3892,33 +3892,33 @@
         <v>1</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I93" s="1"/>
       <c r="K93" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121VMF</v>
+        <v>20211107U11BF</v>
       </c>
       <c r="L93" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211121VWF</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211107U11GF</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>20211121</v>
+        <v>20211107</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -3933,27 +3933,27 @@
         <v>38</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I94" s="1"/>
       <c r="K94" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121OMF</v>
+        <v>20211107U11BE</v>
       </c>
       <c r="L94" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211121OWF</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211107U11GE</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>20211121</v>
+        <v>20211107</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -3968,27 +3968,27 @@
         <v>38</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I95" s="1"/>
       <c r="K95" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121VME</v>
+        <v>20211107U13BF</v>
       </c>
       <c r="L95" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211121VWE</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211107U13GF</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>20211121</v>
+        <v>20211107</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -3997,30 +3997,30 @@
         <v>1</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I96" s="1"/>
       <c r="K96" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211121VMS</v>
+        <v>20211107U15ME</v>
       </c>
       <c r="L96" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20211121VWS</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211107U15WE</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>20211128</v>
+        <v>20211121</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>12</v>
@@ -4029,13 +4029,13 @@
         <v>0</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>19</v>
@@ -4043,34 +4043,34 @@
       <c r="I97" s="1"/>
       <c r="K97" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211128U13TE</v>
+        <v>20211121OME</v>
       </c>
       <c r="L97" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211121OWE</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>20211128</v>
+        <v>20211121</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>19</v>
@@ -4078,34 +4078,34 @@
       <c r="I98" s="1"/>
       <c r="K98" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211128U13TF</v>
+        <v>20211121OMS</v>
       </c>
       <c r="L98" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211121OWS</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>20211128</v>
+        <v>20211121</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D99">
         <v>0</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>19</v>
@@ -4113,19 +4113,19 @@
       <c r="I99" s="1"/>
       <c r="K99" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211128U17TE</v>
+        <v>20211121VMF</v>
       </c>
       <c r="L99" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211121VWF</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>20211128</v>
+        <v>20211121</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>11</v>
@@ -4134,13 +4134,13 @@
         <v>0</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>19</v>
@@ -4148,32 +4148,34 @@
       <c r="I100" s="1"/>
       <c r="K100" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20211128U17TF</v>
+        <v>20211121OMF</v>
       </c>
       <c r="L100" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+        <v>20211121OWF</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>20211128</v>
+        <v>20211121</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C101" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D101">
         <v>0</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>19</v>
@@ -4181,9 +4183,217 @@
       <c r="I101" s="1"/>
       <c r="K101" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20211121VME</v>
+      </c>
+      <c r="L101" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20211121VWE</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>20211121</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I102" s="1"/>
+      <c r="K102" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20211121VMS</v>
+      </c>
+      <c r="L102" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20211121VWS</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>20211128</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I103" s="1"/>
+      <c r="K103" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20211128U13TE</v>
+      </c>
+      <c r="L103" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>20211128</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I104" s="1"/>
+      <c r="K104" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20211128U13TF</v>
+      </c>
+      <c r="L104" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>20211128</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I105" s="1"/>
+      <c r="K105" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20211128U17TE</v>
+      </c>
+      <c r="L105" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>20211128</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I106" s="1"/>
+      <c r="K106" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20211128U17TF</v>
+      </c>
+      <c r="L106" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>20211128</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C107" s="1"/>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I107" s="1"/>
+      <c r="K107" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20211128OT</v>
       </c>
-      <c r="L101" t="str">
+      <c r="L107" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
         <v>N/A</v>
       </c>

</xml_diff>

<commit_message>
format change to SA Schools in dates
</commit_message>
<xml_diff>
--- a/2021/2021FSAdates.xlsx
+++ b/2021/2021FSAdates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\GitHub\FencingSAResults\2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9E5C19-704C-4228-A17B-8F708C9B5465}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EE3542-F93B-4F63-8DCD-7ED7022F5AE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15855" yWindow="-14940" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14235" yWindow="-15540" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -181,9 +181,6 @@
     <t>U17</t>
   </si>
   <si>
-    <t>SASchools</t>
-  </si>
-  <si>
     <t>09:15</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>12:15</t>
+  </si>
+  <si>
+    <t>SA Schools</t>
   </si>
 </sst>
 </file>
@@ -645,9 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD30"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3239,10 +3237,10 @@
         <v>43</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I74" s="1"/>
       <c r="K74" t="str">
@@ -3274,10 +3272,10 @@
         <v>44</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I75" s="1"/>
       <c r="K75" t="str">
@@ -3309,10 +3307,10 @@
         <v>44</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I76" s="1"/>
       <c r="K76" t="str">
@@ -3344,10 +3342,10 @@
         <v>42</v>
       </c>
       <c r="G77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H77" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="I77" s="1"/>
       <c r="K77" t="str">
@@ -3379,10 +3377,10 @@
         <v>42</v>
       </c>
       <c r="G78" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H78" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="I78" s="1"/>
       <c r="K78" t="str">

</xml_diff>